<commit_message>
INTEGRACAO - Express Parte 1
</commit_message>
<xml_diff>
--- a/contas_a_pagar_express/entrada/baixas.xlsx
+++ b/contas_a_pagar_express/entrada/baixas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\18 - DEPARTAMENTO DE PROJETOS\Elder\Importador\Conjunto de Dados\Layouts\Financeiro\_ferramentas\contas_a_pagar_express\entrada\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DO BRASIL " sheetId="1" r:id="rId1"/>
@@ -4094,6 +4099,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4141,7 +4149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4176,7 +4184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4387,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6099,8 +6107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6109,8 +6117,8 @@
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -6138,10 +6146,10 @@
       <c r="D2" s="222" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="222"/>
-      <c r="F2" s="223">
+      <c r="E2" s="223">
         <v>42124</v>
       </c>
+      <c r="F2" s="222"/>
       <c r="G2" s="224"/>
       <c r="H2" s="110" t="s">
         <v>8</v>
@@ -6154,8 +6162,8 @@
       <c r="B3" s="222"/>
       <c r="C3" s="222"/>
       <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="222"/>
       <c r="G3" s="224"/>
       <c r="H3" s="110" t="s">
         <v>8</v>
@@ -6187,10 +6195,10 @@
         <v>77</v>
       </c>
       <c r="E5" s="226" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="226" t="s">
         <v>183</v>
-      </c>
-      <c r="F5" s="226" t="s">
-        <v>57</v>
       </c>
       <c r="G5" s="227"/>
       <c r="H5" s="110" t="s">
@@ -6210,8 +6218,8 @@
       <c r="D6" s="235">
         <v>130</v>
       </c>
-      <c r="E6" s="235"/>
-      <c r="F6" s="238"/>
+      <c r="E6" s="238"/>
+      <c r="F6" s="235"/>
       <c r="G6" s="241"/>
       <c r="H6" s="231" t="s">
         <v>8</v>
@@ -6228,8 +6236,8 @@
       <c r="D7" s="244">
         <v>20</v>
       </c>
-      <c r="E7" s="244"/>
-      <c r="F7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="244"/>
       <c r="G7" s="247"/>
       <c r="H7" s="231" t="s">
         <v>8</v>
@@ -6244,10 +6252,10 @@
       </c>
       <c r="C8" s="249"/>
       <c r="D8" s="250"/>
-      <c r="E8" s="251">
+      <c r="E8" s="246"/>
+      <c r="F8" s="251">
         <v>81</v>
       </c>
-      <c r="F8" s="246"/>
       <c r="G8" s="247"/>
       <c r="H8" s="231" t="s">
         <v>8</v>
@@ -6262,10 +6270,10 @@
       </c>
       <c r="C9" s="245"/>
       <c r="D9" s="252"/>
-      <c r="E9" s="235">
+      <c r="E9" s="253"/>
+      <c r="F9" s="235">
         <v>50.9</v>
       </c>
-      <c r="F9" s="253"/>
       <c r="G9" s="247"/>
       <c r="H9" s="231" t="s">
         <v>8</v>
@@ -6280,10 +6288,10 @@
       </c>
       <c r="C10" s="237"/>
       <c r="D10" s="240"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="253">
+      <c r="E10" s="253">
         <v>256</v>
       </c>
+      <c r="F10" s="235"/>
       <c r="G10" s="247"/>
       <c r="H10" s="231" t="s">
         <v>8</v>
@@ -6294,8 +6302,8 @@
       <c r="B11" s="138"/>
       <c r="C11" s="137"/>
       <c r="D11" s="150"/>
-      <c r="E11" s="153"/>
-      <c r="F11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="153"/>
       <c r="G11" s="158"/>
       <c r="H11" s="110"/>
     </row>
@@ -6308,10 +6316,10 @@
       </c>
       <c r="C12" s="130"/>
       <c r="D12" s="147"/>
-      <c r="E12" s="124">
+      <c r="E12" s="132"/>
+      <c r="F12" s="124">
         <v>64</v>
       </c>
-      <c r="F12" s="132"/>
       <c r="G12" s="161"/>
       <c r="H12" s="110" t="s">
         <v>8</v>
@@ -6330,8 +6338,8 @@
       <c r="D13" s="147">
         <v>134.52000000000001</v>
       </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="124"/>
       <c r="G13" s="161"/>
       <c r="H13" s="110" t="s">
         <v>8</v>
@@ -6350,8 +6358,8 @@
       <c r="D14" s="147">
         <v>500</v>
       </c>
-      <c r="E14" s="124"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="124"/>
       <c r="G14" s="161"/>
       <c r="H14" s="110" t="s">
         <v>8</v>
@@ -6370,8 +6378,8 @@
       <c r="D15" s="147">
         <v>4829.1400000000003</v>
       </c>
-      <c r="E15" s="124"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="161"/>
       <c r="H15" s="110" t="s">
         <v>8</v>
@@ -6388,8 +6396,8 @@
       <c r="D16" s="147">
         <v>1026.33</v>
       </c>
-      <c r="E16" s="124"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="124"/>
       <c r="G16" s="161"/>
       <c r="H16" s="110" t="s">
         <v>8</v>
@@ -6406,8 +6414,8 @@
       <c r="D17" s="147">
         <v>1080</v>
       </c>
-      <c r="E17" s="124"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="124"/>
       <c r="G17" s="161"/>
       <c r="H17" s="110" t="s">
         <v>8</v>
@@ -6424,8 +6432,8 @@
       <c r="D18" s="146">
         <v>331.6</v>
       </c>
-      <c r="E18" s="124"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="124"/>
       <c r="G18" s="161"/>
       <c r="H18" s="110" t="s">
         <v>8</v>
@@ -6440,10 +6448,10 @@
       </c>
       <c r="C19" s="127"/>
       <c r="D19" s="146"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="132">
+      <c r="E19" s="132">
         <v>8000</v>
       </c>
+      <c r="F19" s="124"/>
       <c r="G19" s="161"/>
       <c r="H19" s="110" t="s">
         <v>8</v>
@@ -6458,10 +6466,10 @@
       </c>
       <c r="C20" s="127"/>
       <c r="D20" s="150"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="132">
+      <c r="E20" s="132">
         <v>504</v>
       </c>
+      <c r="F20" s="153"/>
       <c r="G20" s="161"/>
       <c r="H20" s="110" t="s">
         <v>8</v>
@@ -6472,8 +6480,8 @@
       <c r="B21" s="131"/>
       <c r="C21" s="162"/>
       <c r="D21" s="146"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="163"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="124"/>
       <c r="G21" s="161"/>
       <c r="H21" s="110"/>
     </row>
@@ -6490,8 +6498,8 @@
       <c r="D22" s="146">
         <v>565</v>
       </c>
-      <c r="E22" s="124"/>
-      <c r="F22" s="163"/>
+      <c r="E22" s="163"/>
+      <c r="F22" s="124"/>
       <c r="G22" s="161"/>
       <c r="H22" s="110" t="s">
         <v>8</v>
@@ -6502,8 +6510,8 @@
       <c r="B23" s="131"/>
       <c r="C23" s="162"/>
       <c r="D23" s="146"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="163"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="124"/>
       <c r="G23" s="161"/>
       <c r="H23" s="110"/>
     </row>
@@ -6518,8 +6526,8 @@
       <c r="D24" s="165">
         <v>1436.04</v>
       </c>
-      <c r="E24" s="156"/>
-      <c r="F24" s="132"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="156"/>
       <c r="G24" s="161"/>
       <c r="H24" s="110" t="s">
         <v>8</v>
@@ -6536,8 +6544,8 @@
       <c r="D25" s="146">
         <v>1246.73</v>
       </c>
-      <c r="E25" s="124"/>
-      <c r="F25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="124"/>
       <c r="G25" s="161"/>
       <c r="H25" s="110" t="s">
         <v>8</v>
@@ -6554,8 +6562,8 @@
       <c r="D26" s="146">
         <v>4800</v>
       </c>
-      <c r="E26" s="124"/>
-      <c r="F26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="124"/>
       <c r="G26" s="161"/>
       <c r="H26" s="110" t="s">
         <v>8</v>
@@ -6570,10 +6578,10 @@
       </c>
       <c r="C27" s="137"/>
       <c r="D27" s="150"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="132">
+      <c r="E27" s="132">
         <v>11969.57</v>
       </c>
+      <c r="F27" s="153"/>
       <c r="G27" s="161"/>
       <c r="H27" s="110" t="s">
         <v>8</v>
@@ -6584,8 +6592,8 @@
       <c r="B28" s="149"/>
       <c r="C28" s="137"/>
       <c r="D28" s="150"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="210"/>
+      <c r="E28" s="210"/>
+      <c r="F28" s="153"/>
       <c r="G28" s="211"/>
       <c r="H28" s="110"/>
     </row>
@@ -6602,8 +6610,8 @@
       <c r="D29" s="170">
         <v>263.64999999999998</v>
       </c>
-      <c r="E29" s="212"/>
-      <c r="F29" s="213"/>
+      <c r="E29" s="213"/>
+      <c r="F29" s="212"/>
       <c r="G29" s="214"/>
       <c r="H29" s="110" t="s">
         <v>8</v>
@@ -6622,8 +6630,8 @@
       <c r="D30" s="146">
         <v>73.48</v>
       </c>
-      <c r="E30" s="124"/>
-      <c r="F30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="124"/>
       <c r="G30" s="208"/>
       <c r="H30" s="110" t="s">
         <v>8</v>
@@ -6640,8 +6648,8 @@
       <c r="D31" s="146">
         <v>4000</v>
       </c>
-      <c r="E31" s="124"/>
-      <c r="F31" s="159"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="124"/>
       <c r="G31" s="208"/>
       <c r="H31" s="110" t="s">
         <v>8</v>
@@ -6652,8 +6660,8 @@
       <c r="B32" s="131"/>
       <c r="C32" s="128"/>
       <c r="D32" s="146"/>
-      <c r="E32" s="124"/>
-      <c r="F32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="124"/>
       <c r="G32" s="208"/>
       <c r="H32" s="110"/>
     </row>
@@ -6670,8 +6678,8 @@
       <c r="D33" s="146">
         <v>162.49</v>
       </c>
-      <c r="E33" s="124"/>
-      <c r="F33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="124"/>
       <c r="G33" s="208"/>
       <c r="H33" s="110" t="s">
         <v>8</v>
@@ -6690,8 +6698,8 @@
       <c r="D34" s="146">
         <v>135</v>
       </c>
-      <c r="E34" s="124"/>
-      <c r="F34" s="159"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="124"/>
       <c r="G34" s="208"/>
       <c r="H34" s="110" t="s">
         <v>8</v>
@@ -6710,8 +6718,8 @@
       <c r="D35" s="146">
         <v>6700</v>
       </c>
-      <c r="E35" s="124"/>
-      <c r="F35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="124"/>
       <c r="G35" s="208"/>
       <c r="H35" s="110" t="s">
         <v>8</v>
@@ -6728,8 +6736,8 @@
       <c r="D36" s="147">
         <v>100</v>
       </c>
-      <c r="E36" s="124"/>
-      <c r="F36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="124"/>
       <c r="G36" s="208"/>
       <c r="H36" s="110" t="s">
         <v>8</v>
@@ -6744,10 +6752,10 @@
       </c>
       <c r="C37" s="143"/>
       <c r="D37" s="147"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="160">
+      <c r="E37" s="160">
         <v>11000</v>
       </c>
+      <c r="F37" s="124"/>
       <c r="G37" s="208"/>
       <c r="H37" s="110" t="s">
         <v>8</v>
@@ -6764,8 +6772,8 @@
       <c r="D38" s="147">
         <v>4053.43</v>
       </c>
-      <c r="E38" s="124"/>
-      <c r="F38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="124"/>
       <c r="G38" s="208"/>
       <c r="H38" s="110" t="s">
         <v>8</v>
@@ -6776,8 +6784,8 @@
       <c r="B39" s="140"/>
       <c r="C39" s="130"/>
       <c r="D39" s="147"/>
-      <c r="E39" s="124"/>
-      <c r="F39" s="132"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="124"/>
       <c r="G39" s="208"/>
       <c r="H39" s="110"/>
     </row>
@@ -6790,10 +6798,10 @@
       </c>
       <c r="C40" s="130"/>
       <c r="D40" s="147"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="132">
+      <c r="E40" s="132">
         <v>6134.45</v>
       </c>
+      <c r="F40" s="124"/>
       <c r="G40" s="135"/>
       <c r="H40" s="110" t="s">
         <v>8</v>
@@ -6808,10 +6816,10 @@
       </c>
       <c r="C41" s="130"/>
       <c r="D41" s="147"/>
-      <c r="E41" s="124"/>
-      <c r="F41" s="132">
+      <c r="E41" s="132">
         <v>20200</v>
       </c>
+      <c r="F41" s="124"/>
       <c r="G41" s="135"/>
       <c r="H41" s="110" t="s">
         <v>8</v>
@@ -6828,8 +6836,8 @@
       <c r="D42" s="178">
         <v>1908.43</v>
       </c>
-      <c r="E42" s="151"/>
-      <c r="F42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="151"/>
       <c r="G42" s="166"/>
       <c r="H42" s="110" t="s">
         <v>8</v>
@@ -6848,8 +6856,8 @@
       <c r="D43" s="198">
         <v>1062</v>
       </c>
-      <c r="E43" s="151"/>
-      <c r="F43" s="148"/>
+      <c r="E43" s="148"/>
+      <c r="F43" s="151"/>
       <c r="G43" s="166"/>
       <c r="H43" s="110" t="s">
         <v>8</v>
@@ -6868,8 +6876,8 @@
       <c r="D44" s="179">
         <v>625</v>
       </c>
-      <c r="E44" s="151"/>
-      <c r="F44" s="148"/>
+      <c r="E44" s="148"/>
+      <c r="F44" s="151"/>
       <c r="G44" s="166"/>
       <c r="H44" s="110" t="s">
         <v>8</v>
@@ -6888,8 +6896,8 @@
       <c r="D45" s="178">
         <v>119.25</v>
       </c>
-      <c r="E45" s="151"/>
-      <c r="F45" s="148"/>
+      <c r="E45" s="148"/>
+      <c r="F45" s="151"/>
       <c r="G45" s="166"/>
       <c r="H45" s="110" t="s">
         <v>8</v>
@@ -6908,8 +6916,8 @@
       <c r="D46" s="178">
         <v>565</v>
       </c>
-      <c r="E46" s="151"/>
-      <c r="F46" s="148"/>
+      <c r="E46" s="148"/>
+      <c r="F46" s="151"/>
       <c r="G46" s="166"/>
       <c r="H46" s="110" t="s">
         <v>8</v>
@@ -6928,8 +6936,8 @@
       <c r="D47" s="178">
         <v>625</v>
       </c>
-      <c r="E47" s="151"/>
-      <c r="F47" s="148"/>
+      <c r="E47" s="148"/>
+      <c r="F47" s="151"/>
       <c r="G47" s="166"/>
       <c r="H47" s="110" t="s">
         <v>8</v>
@@ -6948,8 +6956,8 @@
       <c r="D48" s="178">
         <v>1569.75</v>
       </c>
-      <c r="E48" s="151"/>
-      <c r="F48" s="148"/>
+      <c r="E48" s="148"/>
+      <c r="F48" s="151"/>
       <c r="G48" s="166"/>
       <c r="H48" s="110" t="s">
         <v>8</v>
@@ -6968,8 +6976,8 @@
       <c r="D49" s="178">
         <v>1431.75</v>
       </c>
-      <c r="E49" s="151"/>
-      <c r="F49" s="148"/>
+      <c r="E49" s="148"/>
+      <c r="F49" s="151"/>
       <c r="G49" s="166"/>
       <c r="H49" s="110" t="s">
         <v>8</v>
@@ -6988,8 +6996,8 @@
       <c r="D50" s="178">
         <v>4819.5</v>
       </c>
-      <c r="E50" s="151"/>
-      <c r="F50" s="148"/>
+      <c r="E50" s="148"/>
+      <c r="F50" s="151"/>
       <c r="G50" s="166"/>
       <c r="H50" s="110" t="s">
         <v>8</v>
@@ -7008,8 +7016,8 @@
       <c r="D51" s="178">
         <v>1076.25</v>
       </c>
-      <c r="E51" s="151"/>
-      <c r="F51" s="148"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="151"/>
       <c r="G51" s="166"/>
       <c r="H51" s="110" t="s">
         <v>8</v>
@@ -7028,8 +7036,8 @@
       <c r="D52" s="178">
         <v>1076.25</v>
       </c>
-      <c r="E52" s="151"/>
-      <c r="F52" s="148"/>
+      <c r="E52" s="148"/>
+      <c r="F52" s="151"/>
       <c r="G52" s="166"/>
       <c r="H52" s="110" t="s">
         <v>8</v>
@@ -7046,8 +7054,8 @@
       <c r="D53" s="116">
         <v>11300</v>
       </c>
-      <c r="E53" s="151"/>
-      <c r="F53" s="148"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="151"/>
       <c r="G53" s="166"/>
       <c r="H53" s="110" t="s">
         <v>8</v>
@@ -7058,8 +7066,8 @@
       <c r="B54" s="133"/>
       <c r="C54" s="128"/>
       <c r="D54" s="116"/>
-      <c r="E54" s="151"/>
-      <c r="F54" s="148"/>
+      <c r="E54" s="148"/>
+      <c r="F54" s="151"/>
       <c r="G54" s="166"/>
       <c r="H54" s="110"/>
     </row>
@@ -7074,8 +7082,8 @@
       <c r="D55" s="116">
         <v>1800</v>
       </c>
-      <c r="E55" s="151"/>
-      <c r="F55" s="148"/>
+      <c r="E55" s="148"/>
+      <c r="F55" s="151"/>
       <c r="G55" s="166"/>
       <c r="H55" s="110" t="s">
         <v>8</v>
@@ -7090,10 +7098,10 @@
       </c>
       <c r="C56" s="128"/>
       <c r="D56" s="116"/>
-      <c r="E56" s="151"/>
-      <c r="F56" s="151">
+      <c r="E56" s="151">
         <v>25</v>
       </c>
+      <c r="F56" s="151"/>
       <c r="G56" s="166"/>
       <c r="H56" s="110" t="s">
         <v>8</v>
@@ -7108,10 +7116,10 @@
       </c>
       <c r="C57" s="128"/>
       <c r="D57" s="116"/>
-      <c r="E57" s="151"/>
-      <c r="F57" s="151">
+      <c r="E57" s="151">
         <v>1600</v>
       </c>
+      <c r="F57" s="151"/>
       <c r="G57" s="166"/>
       <c r="H57" s="110" t="s">
         <v>8</v>
@@ -7122,8 +7130,8 @@
       <c r="B58" s="133"/>
       <c r="C58" s="128"/>
       <c r="D58" s="116"/>
-      <c r="E58" s="151"/>
-      <c r="F58" s="148"/>
+      <c r="E58" s="148"/>
+      <c r="F58" s="151"/>
       <c r="G58" s="166"/>
       <c r="H58" s="110"/>
     </row>
@@ -7140,8 +7148,8 @@
       <c r="D59" s="198">
         <v>1735.36</v>
       </c>
-      <c r="E59" s="181"/>
-      <c r="F59" s="148"/>
+      <c r="E59" s="148"/>
+      <c r="F59" s="181"/>
       <c r="G59" s="166"/>
       <c r="H59" s="110" t="s">
         <v>8</v>
@@ -7160,8 +7168,8 @@
       <c r="D60" s="198">
         <v>170.2</v>
       </c>
-      <c r="E60" s="151"/>
-      <c r="F60" s="148"/>
+      <c r="E60" s="148"/>
+      <c r="F60" s="151"/>
       <c r="G60" s="166"/>
       <c r="H60" s="110" t="s">
         <v>8</v>
@@ -7180,8 +7188,8 @@
       <c r="D61" s="198">
         <v>113.32</v>
       </c>
-      <c r="E61" s="151"/>
-      <c r="F61" s="148"/>
+      <c r="E61" s="148"/>
+      <c r="F61" s="151"/>
       <c r="G61" s="166"/>
       <c r="H61" s="110" t="s">
         <v>8</v>
@@ -7200,8 +7208,8 @@
       <c r="D62" s="198">
         <v>605.28</v>
       </c>
-      <c r="E62" s="122"/>
-      <c r="F62" s="148"/>
+      <c r="E62" s="148"/>
+      <c r="F62" s="122"/>
       <c r="G62" s="166"/>
       <c r="H62" s="110" t="s">
         <v>8</v>
@@ -7220,8 +7228,8 @@
       <c r="D63" s="198">
         <v>1536</v>
       </c>
-      <c r="E63" s="181"/>
-      <c r="F63" s="148"/>
+      <c r="E63" s="148"/>
+      <c r="F63" s="181"/>
       <c r="G63" s="166"/>
       <c r="H63" s="110" t="s">
         <v>8</v>
@@ -7238,8 +7246,8 @@
       <c r="D64" s="198">
         <v>5350</v>
       </c>
-      <c r="E64" s="181"/>
-      <c r="F64" s="148"/>
+      <c r="E64" s="148"/>
+      <c r="F64" s="181"/>
       <c r="G64" s="166"/>
       <c r="H64" s="110" t="s">
         <v>8</v>
@@ -7256,8 +7264,8 @@
       <c r="D65" s="198">
         <v>200</v>
       </c>
-      <c r="E65" s="181"/>
-      <c r="F65" s="148"/>
+      <c r="E65" s="148"/>
+      <c r="F65" s="181"/>
       <c r="G65" s="166"/>
       <c r="H65" s="110" t="s">
         <v>8</v>
@@ -7272,10 +7280,10 @@
       </c>
       <c r="C66" s="177"/>
       <c r="D66" s="182"/>
-      <c r="E66" s="122"/>
-      <c r="F66" s="121">
+      <c r="E66" s="121">
         <v>11642.7</v>
       </c>
+      <c r="F66" s="122"/>
       <c r="G66" s="166"/>
       <c r="H66" s="110" t="s">
         <v>8</v>
@@ -7286,8 +7294,8 @@
       <c r="B67" s="176"/>
       <c r="C67" s="177"/>
       <c r="D67" s="185"/>
-      <c r="E67" s="122"/>
-      <c r="F67" s="121"/>
+      <c r="E67" s="121"/>
+      <c r="F67" s="122"/>
       <c r="G67" s="166"/>
       <c r="H67" s="110"/>
     </row>
@@ -7304,8 +7312,8 @@
       <c r="D68" s="182">
         <v>2734.4</v>
       </c>
-      <c r="E68" s="122"/>
-      <c r="F68" s="148"/>
+      <c r="E68" s="148"/>
+      <c r="F68" s="122"/>
       <c r="G68" s="166"/>
       <c r="H68" s="110" t="s">
         <v>8</v>
@@ -7324,8 +7332,8 @@
       <c r="D69" s="198">
         <v>3712.35</v>
       </c>
-      <c r="E69" s="181"/>
-      <c r="F69" s="148"/>
+      <c r="E69" s="148"/>
+      <c r="F69" s="181"/>
       <c r="G69" s="166"/>
       <c r="H69" s="110" t="s">
         <v>8</v>
@@ -7344,8 +7352,8 @@
       <c r="D70" s="198">
         <v>4833.96</v>
       </c>
-      <c r="E70" s="181"/>
-      <c r="F70" s="148"/>
+      <c r="E70" s="148"/>
+      <c r="F70" s="181"/>
       <c r="G70" s="166"/>
       <c r="H70" s="110" t="s">
         <v>8</v>
@@ -7364,8 +7372,8 @@
       <c r="D71" s="198">
         <v>3712.35</v>
       </c>
-      <c r="E71" s="181"/>
-      <c r="F71" s="148"/>
+      <c r="E71" s="148"/>
+      <c r="F71" s="181"/>
       <c r="G71" s="166"/>
       <c r="H71" s="110" t="s">
         <v>8</v>
@@ -7382,8 +7390,8 @@
       <c r="D72" s="198">
         <v>4604</v>
       </c>
-      <c r="E72" s="122"/>
-      <c r="F72" s="148"/>
+      <c r="E72" s="148"/>
+      <c r="F72" s="122"/>
       <c r="G72" s="166"/>
       <c r="H72" s="110" t="s">
         <v>8</v>
@@ -7400,8 +7408,8 @@
       <c r="D73" s="186">
         <v>390</v>
       </c>
-      <c r="E73" s="122"/>
-      <c r="F73" s="148"/>
+      <c r="E73" s="148"/>
+      <c r="F73" s="122"/>
       <c r="G73" s="166"/>
       <c r="H73" s="110" t="s">
         <v>8</v>
@@ -7416,10 +7424,10 @@
       </c>
       <c r="C74" s="136"/>
       <c r="D74" s="184"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="171">
+      <c r="E74" s="171">
         <v>17184.759999999998</v>
       </c>
+      <c r="F74" s="126"/>
       <c r="G74" s="197"/>
       <c r="H74" s="152" t="s">
         <v>8</v>
@@ -7434,10 +7442,10 @@
       </c>
       <c r="C75" s="183"/>
       <c r="D75" s="198"/>
-      <c r="E75" s="181"/>
-      <c r="F75" s="121">
+      <c r="E75" s="121">
         <v>390</v>
       </c>
+      <c r="F75" s="181"/>
       <c r="G75" s="166"/>
       <c r="H75" s="110" t="s">
         <v>8</v>
@@ -7452,10 +7460,10 @@
       </c>
       <c r="C76" s="183"/>
       <c r="D76" s="198"/>
-      <c r="E76" s="181"/>
-      <c r="F76" s="132">
+      <c r="E76" s="132">
         <v>449</v>
       </c>
+      <c r="F76" s="181"/>
       <c r="G76" s="135"/>
       <c r="H76" s="110" t="s">
         <v>8</v>
@@ -7466,8 +7474,8 @@
       <c r="B77" s="177"/>
       <c r="C77" s="183"/>
       <c r="D77" s="198"/>
-      <c r="E77" s="181"/>
-      <c r="F77" s="132"/>
+      <c r="E77" s="132"/>
+      <c r="F77" s="181"/>
       <c r="G77" s="208"/>
       <c r="H77" s="110"/>
     </row>
@@ -7482,8 +7490,8 @@
       <c r="D78" s="181">
         <v>9300</v>
       </c>
-      <c r="E78" s="181"/>
-      <c r="F78" s="132"/>
+      <c r="E78" s="132"/>
+      <c r="F78" s="181"/>
       <c r="G78" s="208"/>
       <c r="H78" s="110" t="s">
         <v>8</v>
@@ -7498,10 +7506,10 @@
       </c>
       <c r="C79" s="175"/>
       <c r="D79" s="198"/>
-      <c r="E79" s="181"/>
-      <c r="F79" s="132">
+      <c r="E79" s="132">
         <v>9300</v>
       </c>
+      <c r="F79" s="181"/>
       <c r="G79" s="208"/>
       <c r="H79" s="110" t="s">
         <v>8</v>
@@ -7512,8 +7520,8 @@
       <c r="B80" s="174"/>
       <c r="C80" s="175"/>
       <c r="D80" s="198"/>
-      <c r="E80" s="181"/>
-      <c r="F80" s="132"/>
+      <c r="E80" s="132"/>
+      <c r="F80" s="181"/>
       <c r="G80" s="208"/>
       <c r="H80" s="110"/>
     </row>
@@ -7526,10 +7534,10 @@
       </c>
       <c r="C81" s="199"/>
       <c r="D81" s="198"/>
-      <c r="E81" s="181"/>
-      <c r="F81" s="132">
+      <c r="E81" s="132">
         <v>217</v>
       </c>
+      <c r="F81" s="181"/>
       <c r="G81" s="208"/>
       <c r="H81" s="110" t="s">
         <v>8</v>
@@ -7548,8 +7556,8 @@
       <c r="D82" s="198">
         <v>2450</v>
       </c>
-      <c r="E82" s="181"/>
-      <c r="F82" s="132"/>
+      <c r="E82" s="132"/>
+      <c r="F82" s="181"/>
       <c r="G82" s="208"/>
       <c r="H82" s="110" t="s">
         <v>8</v>
@@ -7564,10 +7572,10 @@
       </c>
       <c r="C83" s="199"/>
       <c r="D83" s="198"/>
-      <c r="E83" s="181"/>
-      <c r="F83" s="132">
+      <c r="E83" s="132">
         <v>2250</v>
       </c>
+      <c r="F83" s="181"/>
       <c r="G83" s="208"/>
       <c r="H83" s="110" t="s">
         <v>8</v>
@@ -7578,8 +7586,8 @@
       <c r="B84" s="176"/>
       <c r="C84" s="199"/>
       <c r="D84" s="198"/>
-      <c r="E84" s="181"/>
-      <c r="F84" s="132"/>
+      <c r="E84" s="132"/>
+      <c r="F84" s="181"/>
       <c r="G84" s="208"/>
       <c r="H84" s="110"/>
     </row>
@@ -7592,10 +7600,10 @@
       </c>
       <c r="C85" s="199"/>
       <c r="D85" s="198"/>
-      <c r="E85" s="181">
+      <c r="E85" s="132"/>
+      <c r="F85" s="181">
         <v>0.35</v>
       </c>
-      <c r="F85" s="132"/>
       <c r="G85" s="208"/>
       <c r="H85" s="110" t="s">
         <v>8</v>
@@ -7606,8 +7614,8 @@
       <c r="B86" s="190"/>
       <c r="C86" s="192"/>
       <c r="D86" s="191"/>
-      <c r="E86" s="193"/>
-      <c r="F86" s="157"/>
+      <c r="E86" s="157"/>
+      <c r="F86" s="193"/>
       <c r="G86" s="215"/>
       <c r="H86" s="111"/>
     </row>
@@ -7616,8 +7624,8 @@
       <c r="B87" s="190"/>
       <c r="C87" s="192"/>
       <c r="D87" s="191"/>
-      <c r="E87" s="193"/>
-      <c r="F87" s="157"/>
+      <c r="E87" s="157"/>
+      <c r="F87" s="193"/>
       <c r="G87" s="215"/>
       <c r="H87" s="111"/>
     </row>
@@ -7632,8 +7640,8 @@
       <c r="D88" s="194">
         <v>4635.3999999999996</v>
       </c>
-      <c r="E88" s="181"/>
-      <c r="F88" s="132"/>
+      <c r="E88" s="132"/>
+      <c r="F88" s="181"/>
       <c r="G88" s="208"/>
       <c r="H88" s="110" t="s">
         <v>8</v>
@@ -7652,8 +7660,8 @@
       <c r="D89" s="194">
         <v>785.81</v>
       </c>
-      <c r="E89" s="181"/>
-      <c r="F89" s="132"/>
+      <c r="E89" s="132"/>
+      <c r="F89" s="181"/>
       <c r="G89" s="208"/>
       <c r="H89" s="110" t="s">
         <v>8</v>
@@ -7672,8 +7680,8 @@
       <c r="D90" s="194">
         <v>73.48</v>
       </c>
-      <c r="E90" s="181"/>
-      <c r="F90" s="132"/>
+      <c r="E90" s="132"/>
+      <c r="F90" s="181"/>
       <c r="G90" s="208"/>
       <c r="H90" s="110" t="s">
         <v>8</v>
@@ -7692,8 +7700,8 @@
       <c r="D91" s="194">
         <v>3300</v>
       </c>
-      <c r="E91" s="181"/>
-      <c r="F91" s="132"/>
+      <c r="E91" s="132"/>
+      <c r="F91" s="181"/>
       <c r="G91" s="208"/>
       <c r="H91" s="110" t="s">
         <v>8</v>
@@ -7708,10 +7716,10 @@
       </c>
       <c r="C92" s="199"/>
       <c r="D92" s="198"/>
-      <c r="E92" s="181"/>
-      <c r="F92" s="132">
+      <c r="E92" s="132">
         <v>7933.33</v>
       </c>
+      <c r="F92" s="181"/>
       <c r="G92" s="208"/>
       <c r="H92" s="110" t="s">
         <v>8</v>
@@ -7726,10 +7734,10 @@
       </c>
       <c r="C93" s="199"/>
       <c r="D93" s="198"/>
-      <c r="E93" s="181"/>
-      <c r="F93" s="132">
+      <c r="E93" s="132">
         <v>3141.45</v>
       </c>
+      <c r="F93" s="181"/>
       <c r="G93" s="208"/>
       <c r="H93" s="110" t="s">
         <v>8</v>
@@ -7744,10 +7752,10 @@
       </c>
       <c r="C94" s="199"/>
       <c r="D94" s="198"/>
-      <c r="E94" s="181"/>
-      <c r="F94" s="132">
+      <c r="E94" s="132">
         <v>179.4</v>
       </c>
+      <c r="F94" s="181"/>
       <c r="G94" s="208"/>
       <c r="H94" s="111" t="s">
         <v>8</v>
@@ -7764,8 +7772,8 @@
       <c r="D95" s="198">
         <v>50.9</v>
       </c>
-      <c r="E95" s="181"/>
-      <c r="F95" s="132"/>
+      <c r="E95" s="132"/>
+      <c r="F95" s="181"/>
       <c r="G95" s="208"/>
       <c r="H95" s="111" t="s">
         <v>8</v>
@@ -7782,8 +7790,8 @@
       <c r="D96" s="198">
         <v>81</v>
       </c>
-      <c r="E96" s="181"/>
-      <c r="F96" s="132"/>
+      <c r="E96" s="132"/>
+      <c r="F96" s="181"/>
       <c r="G96" s="208"/>
       <c r="H96" s="111" t="s">
         <v>8</v>
@@ -7794,8 +7802,8 @@
       <c r="B97" s="176"/>
       <c r="C97" s="199"/>
       <c r="D97" s="198"/>
-      <c r="E97" s="181"/>
-      <c r="F97" s="132"/>
+      <c r="E97" s="132"/>
+      <c r="F97" s="181"/>
       <c r="G97" s="208"/>
       <c r="H97" s="111"/>
     </row>
@@ -7810,8 +7818,8 @@
       <c r="D98" s="198">
         <v>1000</v>
       </c>
-      <c r="E98" s="181"/>
-      <c r="F98" s="132"/>
+      <c r="E98" s="132"/>
+      <c r="F98" s="181"/>
       <c r="G98" s="208"/>
       <c r="H98" s="111" t="s">
         <v>8</v>
@@ -7830,8 +7838,8 @@
       <c r="D99" s="194">
         <v>3500</v>
       </c>
-      <c r="E99" s="181"/>
-      <c r="F99" s="132"/>
+      <c r="E99" s="132"/>
+      <c r="F99" s="181"/>
       <c r="G99" s="208"/>
       <c r="H99" s="111" t="s">
         <v>8</v>
@@ -7850,8 +7858,8 @@
       <c r="D100" s="194">
         <v>765</v>
       </c>
-      <c r="E100" s="181"/>
-      <c r="F100" s="132"/>
+      <c r="E100" s="132"/>
+      <c r="F100" s="181"/>
       <c r="G100" s="208"/>
       <c r="H100" s="111" t="s">
         <v>8</v>
@@ -7868,8 +7876,8 @@
       <c r="D101" s="194">
         <v>100</v>
       </c>
-      <c r="E101" s="181"/>
-      <c r="F101" s="132"/>
+      <c r="E101" s="132"/>
+      <c r="F101" s="181"/>
       <c r="G101" s="208"/>
       <c r="H101" s="111" t="s">
         <v>8</v>
@@ -7884,10 +7892,10 @@
       </c>
       <c r="C102" s="175"/>
       <c r="D102" s="194"/>
-      <c r="E102" s="181"/>
-      <c r="F102" s="132">
+      <c r="E102" s="132">
         <v>3252</v>
       </c>
+      <c r="F102" s="181"/>
       <c r="G102" s="208"/>
       <c r="H102" s="111" t="s">
         <v>8</v>
@@ -7898,8 +7906,8 @@
       <c r="B103" s="174"/>
       <c r="C103" s="175"/>
       <c r="D103" s="194"/>
-      <c r="E103" s="114"/>
-      <c r="F103" s="172"/>
+      <c r="E103" s="172"/>
+      <c r="F103" s="114"/>
       <c r="G103" s="209"/>
       <c r="H103" s="110"/>
     </row>
@@ -7916,8 +7924,8 @@
       <c r="D104" s="196">
         <v>3500</v>
       </c>
-      <c r="E104" s="122"/>
-      <c r="F104" s="172"/>
+      <c r="E104" s="172"/>
+      <c r="F104" s="122"/>
       <c r="G104" s="209"/>
       <c r="H104" s="111" t="s">
         <v>8</v>
@@ -7934,8 +7942,8 @@
       <c r="D105" s="194">
         <v>6000</v>
       </c>
-      <c r="E105" s="114"/>
-      <c r="F105" s="172"/>
+      <c r="E105" s="172"/>
+      <c r="F105" s="114"/>
       <c r="G105" s="209"/>
       <c r="H105" s="111" t="s">
         <v>8</v>
@@ -7950,10 +7958,10 @@
       </c>
       <c r="C106" s="175"/>
       <c r="D106" s="194"/>
-      <c r="E106" s="114"/>
-      <c r="F106" s="172">
+      <c r="E106" s="172">
         <v>9300</v>
       </c>
+      <c r="F106" s="114"/>
       <c r="G106" s="209"/>
       <c r="H106" s="111" t="s">
         <v>8</v>
@@ -7968,10 +7976,10 @@
       </c>
       <c r="C107" s="175"/>
       <c r="D107" s="194"/>
-      <c r="E107" s="114"/>
-      <c r="F107" s="172">
+      <c r="E107" s="172">
         <v>25</v>
       </c>
+      <c r="F107" s="114"/>
       <c r="G107" s="209"/>
       <c r="H107" s="111" t="s">
         <v>8</v>
@@ -7982,8 +7990,8 @@
       <c r="B108" s="174"/>
       <c r="C108" s="175"/>
       <c r="D108" s="194"/>
-      <c r="E108" s="114"/>
-      <c r="F108" s="172"/>
+      <c r="E108" s="172"/>
+      <c r="F108" s="114"/>
       <c r="G108" s="209"/>
       <c r="H108" s="110"/>
     </row>
@@ -7998,8 +8006,8 @@
       <c r="D109" s="198">
         <v>50</v>
       </c>
-      <c r="E109" s="114"/>
-      <c r="F109" s="172"/>
+      <c r="E109" s="172"/>
+      <c r="F109" s="114"/>
       <c r="G109" s="209"/>
       <c r="H109" s="111" t="s">
         <v>8</v>
@@ -8010,8 +8018,8 @@
       <c r="B110" s="174"/>
       <c r="C110" s="175"/>
       <c r="D110" s="194"/>
-      <c r="E110" s="114"/>
-      <c r="F110" s="172"/>
+      <c r="E110" s="172"/>
+      <c r="F110" s="114"/>
       <c r="G110" s="209"/>
       <c r="H110" s="110"/>
     </row>
@@ -8026,8 +8034,8 @@
       <c r="D111" s="194">
         <v>6350</v>
       </c>
-      <c r="E111" s="114"/>
-      <c r="F111" s="172"/>
+      <c r="E111" s="172"/>
+      <c r="F111" s="114"/>
       <c r="G111" s="209"/>
       <c r="H111" s="111" t="s">
         <v>8</v>
@@ -8042,10 +8050,10 @@
       </c>
       <c r="C112" s="175"/>
       <c r="D112" s="194"/>
-      <c r="E112" s="114"/>
-      <c r="F112" s="172">
+      <c r="E112" s="172">
         <v>6352.04</v>
       </c>
+      <c r="F112" s="114"/>
       <c r="G112" s="209"/>
       <c r="H112" s="111" t="s">
         <v>8</v>
@@ -8056,8 +8064,8 @@
       <c r="B113" s="174"/>
       <c r="C113" s="175"/>
       <c r="D113" s="194"/>
-      <c r="E113" s="114"/>
-      <c r="F113" s="172"/>
+      <c r="E113" s="172"/>
+      <c r="F113" s="114"/>
       <c r="G113" s="209"/>
       <c r="H113" s="110"/>
     </row>
@@ -8072,8 +8080,8 @@
       <c r="D114" s="198">
         <v>2450</v>
       </c>
-      <c r="E114" s="114"/>
-      <c r="F114" s="172"/>
+      <c r="E114" s="172"/>
+      <c r="F114" s="114"/>
       <c r="G114" s="209"/>
       <c r="H114" s="110" t="s">
         <v>8</v>
@@ -8090,8 +8098,8 @@
       <c r="D115" s="198">
         <v>2120</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="172"/>
+      <c r="E115" s="172"/>
+      <c r="F115" s="114"/>
       <c r="G115" s="209"/>
       <c r="H115" s="110" t="s">
         <v>8</v>
@@ -8106,10 +8114,10 @@
       </c>
       <c r="C116" s="199"/>
       <c r="D116" s="198"/>
-      <c r="E116" s="114"/>
-      <c r="F116" s="172">
+      <c r="E116" s="172">
         <v>4600</v>
       </c>
+      <c r="F116" s="114"/>
       <c r="G116" s="209"/>
       <c r="H116" s="110" t="s">
         <v>8</v>
@@ -8120,8 +8128,8 @@
       <c r="B117" s="174"/>
       <c r="C117" s="199"/>
       <c r="D117" s="198"/>
-      <c r="E117" s="114"/>
-      <c r="F117" s="172"/>
+      <c r="E117" s="172"/>
+      <c r="F117" s="114"/>
       <c r="G117" s="209"/>
       <c r="H117" s="110"/>
     </row>
@@ -8134,10 +8142,10 @@
       </c>
       <c r="C118" s="199"/>
       <c r="D118" s="198"/>
-      <c r="E118" s="114">
+      <c r="E118" s="172"/>
+      <c r="F118" s="114">
         <v>0.35</v>
       </c>
-      <c r="F118" s="172"/>
       <c r="G118" s="209"/>
       <c r="H118" s="110" t="s">
         <v>8</v>
@@ -8148,8 +8156,8 @@
       <c r="B119" s="176"/>
       <c r="C119" s="199"/>
       <c r="D119" s="198"/>
-      <c r="E119" s="114"/>
-      <c r="F119" s="172"/>
+      <c r="E119" s="172"/>
+      <c r="F119" s="114"/>
       <c r="G119" s="209"/>
       <c r="H119" s="110"/>
     </row>
@@ -8166,8 +8174,8 @@
       <c r="D120" s="198">
         <v>2450</v>
       </c>
-      <c r="E120" s="168"/>
-      <c r="F120" s="134"/>
+      <c r="E120" s="134"/>
+      <c r="F120" s="168"/>
       <c r="G120" s="144"/>
       <c r="H120" s="110" t="s">
         <v>8</v>
@@ -8182,10 +8190,10 @@
       </c>
       <c r="C121" s="175"/>
       <c r="D121" s="198"/>
-      <c r="E121" s="168"/>
-      <c r="F121" s="145">
+      <c r="E121" s="145">
         <v>10.5</v>
       </c>
+      <c r="F121" s="168"/>
       <c r="G121" s="216"/>
       <c r="H121" s="110" t="s">
         <v>8</v>
@@ -8196,8 +8204,8 @@
       <c r="B122" s="176"/>
       <c r="C122" s="199"/>
       <c r="D122" s="198"/>
-      <c r="E122" s="114"/>
-      <c r="F122" s="172"/>
+      <c r="E122" s="172"/>
+      <c r="F122" s="114"/>
       <c r="G122" s="209"/>
       <c r="H122" s="110"/>
     </row>
@@ -8210,10 +8218,10 @@
       </c>
       <c r="C123" s="199"/>
       <c r="D123" s="198"/>
-      <c r="E123" s="114">
+      <c r="E123" s="172"/>
+      <c r="F123" s="114">
         <v>62.5</v>
       </c>
-      <c r="F123" s="172"/>
       <c r="G123" s="209"/>
       <c r="H123" s="110" t="s">
         <v>8</v>
@@ -8230,8 +8238,8 @@
       <c r="D124" s="205">
         <v>3800</v>
       </c>
-      <c r="E124" s="206"/>
-      <c r="F124" s="204"/>
+      <c r="E124" s="204"/>
+      <c r="F124" s="206"/>
       <c r="G124" s="217"/>
       <c r="H124" s="110" t="s">
         <v>8</v>
@@ -8248,8 +8256,8 @@
       <c r="D125" s="205">
         <v>390</v>
       </c>
-      <c r="E125" s="206"/>
-      <c r="F125" s="204"/>
+      <c r="E125" s="204"/>
+      <c r="F125" s="206"/>
       <c r="G125" s="217"/>
       <c r="H125" s="110" t="s">
         <v>8</v>
@@ -8264,10 +8272,10 @@
       </c>
       <c r="C126" s="202"/>
       <c r="D126" s="205"/>
-      <c r="E126" s="206"/>
-      <c r="F126" s="204">
+      <c r="E126" s="204">
         <v>6511.85</v>
       </c>
+      <c r="F126" s="206"/>
       <c r="G126" s="217"/>
       <c r="H126" s="110" t="s">
         <v>8</v>
@@ -8282,10 +8290,10 @@
       </c>
       <c r="C127" s="199"/>
       <c r="D127" s="198"/>
-      <c r="E127" s="114"/>
-      <c r="F127" s="172">
+      <c r="E127" s="172">
         <v>120</v>
       </c>
+      <c r="F127" s="114"/>
       <c r="G127" s="209"/>
       <c r="H127" s="110" t="s">
         <v>8</v>
@@ -8296,8 +8304,8 @@
       <c r="B128" s="176"/>
       <c r="C128" s="199"/>
       <c r="D128" s="198"/>
-      <c r="E128" s="114"/>
-      <c r="F128" s="172"/>
+      <c r="E128" s="172"/>
+      <c r="F128" s="114"/>
       <c r="G128" s="209"/>
       <c r="H128" s="110"/>
     </row>
@@ -8310,10 +8318,10 @@
       </c>
       <c r="C129" s="175"/>
       <c r="D129" s="178"/>
-      <c r="E129" s="168"/>
-      <c r="F129" s="132">
+      <c r="E129" s="132">
         <v>20</v>
       </c>
+      <c r="F129" s="168"/>
       <c r="G129" s="144"/>
       <c r="H129" s="110" t="s">
         <v>8</v>
@@ -8324,8 +8332,8 @@
       <c r="B130" s="176"/>
       <c r="C130" s="199"/>
       <c r="D130" s="198"/>
-      <c r="E130" s="114"/>
-      <c r="F130" s="172"/>
+      <c r="E130" s="172"/>
+      <c r="F130" s="114"/>
       <c r="G130" s="209"/>
       <c r="H130" s="110"/>
     </row>
@@ -8340,8 +8348,8 @@
       <c r="D131" s="198">
         <v>10</v>
       </c>
-      <c r="E131" s="114"/>
-      <c r="F131" s="172"/>
+      <c r="E131" s="172"/>
+      <c r="F131" s="114"/>
       <c r="G131" s="209"/>
       <c r="H131" s="110" t="s">
         <v>8</v>
@@ -8356,10 +8364,10 @@
       </c>
       <c r="C132" s="199"/>
       <c r="D132" s="198"/>
-      <c r="E132" s="114"/>
-      <c r="F132" s="172">
+      <c r="E132" s="172">
         <v>20</v>
       </c>
+      <c r="F132" s="114"/>
       <c r="G132" s="209"/>
       <c r="H132" s="110" t="s">
         <v>25</v>
@@ -8370,8 +8378,8 @@
       <c r="B133" s="203"/>
       <c r="C133" s="202"/>
       <c r="D133" s="205"/>
-      <c r="E133" s="206"/>
-      <c r="F133" s="204"/>
+      <c r="E133" s="204"/>
+      <c r="F133" s="206"/>
       <c r="G133" s="217"/>
       <c r="H133" s="187"/>
     </row>
@@ -8386,8 +8394,8 @@
       <c r="D134" s="205">
         <v>210</v>
       </c>
-      <c r="E134" s="206"/>
-      <c r="F134" s="204"/>
+      <c r="E134" s="204"/>
+      <c r="F134" s="206"/>
       <c r="G134" s="217"/>
       <c r="H134" s="110" t="s">
         <v>8</v>
@@ -8402,10 +8410,10 @@
       </c>
       <c r="C135" s="199"/>
       <c r="D135" s="198"/>
-      <c r="E135" s="114"/>
-      <c r="F135" s="172">
+      <c r="E135" s="172">
         <v>572</v>
       </c>
+      <c r="F135" s="114"/>
       <c r="G135" s="209"/>
       <c r="H135" s="110" t="s">
         <v>25</v>
@@ -8420,10 +8428,10 @@
       </c>
       <c r="C136" s="199"/>
       <c r="D136" s="198"/>
-      <c r="E136" s="114">
+      <c r="E136" s="172"/>
+      <c r="F136" s="114">
         <v>62</v>
       </c>
-      <c r="F136" s="172"/>
       <c r="G136" s="209"/>
       <c r="H136" s="110" t="s">
         <v>8</v>
@@ -8439,7 +8447,7 @@
   <dimension ref="A1:G324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13872,8 +13880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14601,7 +14609,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15024,8 +15032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>